<commit_message>
add router rip and subinterfaces
</commit_message>
<xml_diff>
--- a/VLSM-VLAN-WAN-CASO-ESTUDIO.xlsx
+++ b/VLSM-VLAN-WAN-CASO-ESTUDIO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Octavo-Semestre\Redes\Caso_De_Estudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB433474-4605-4FC2-9E86-59C5C51A9CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8BDAEA-0A4A-4569-B1B5-00B4598E8875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{70712092-6E08-405F-915F-8AB6473FB4D8}"/>
+    <workbookView xWindow="285" yWindow="435" windowWidth="20205" windowHeight="10365" xr2:uid="{70712092-6E08-405F-915F-8AB6473FB4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
add dhcp in routers
</commit_message>
<xml_diff>
--- a/VLSM-VLAN-WAN-CASO-ESTUDIO.xlsx
+++ b/VLSM-VLAN-WAN-CASO-ESTUDIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Octavo-Semestre\Redes\Caso_De_Estudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCF7390-12B7-4482-888B-B831700A242A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C4FC34-C679-4AD2-A032-0F96FD75EB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="435" windowWidth="20205" windowHeight="10365" xr2:uid="{70712092-6E08-405F-915F-8AB6473FB4D8}"/>
   </bookViews>
@@ -218,24 +218,12 @@
     <t>Servidores-Pereira</t>
   </si>
   <si>
-    <t>10.3.191.127</t>
-  </si>
-  <si>
     <t>10.3.192.1</t>
   </si>
   <si>
-    <t>10.3.191.126</t>
-  </si>
-  <si>
     <t>10.3.192.129</t>
   </si>
   <si>
-    <t>10.3.191.191</t>
-  </si>
-  <si>
-    <t>10.3.191.190</t>
-  </si>
-  <si>
     <t>10.3.63.254</t>
   </si>
   <si>
@@ -288,6 +276,18 @@
   </si>
   <si>
     <t>37.0.0.11</t>
+  </si>
+  <si>
+    <t>10.3.192.126</t>
+  </si>
+  <si>
+    <t>10.3.192.127</t>
+  </si>
+  <si>
+    <t>10.3.192.190</t>
+  </si>
+  <si>
+    <t>10.3.192.191</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,353 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -389,6 +735,54 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC2BF242-74B9-4E4B-B03C-42020D7FDC01}" name="Tabla1" displayName="Tabla1" ref="B4:H15" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
+  <autoFilter ref="B4:H15" xr:uid="{DC2BF242-74B9-4E4B-B03C-42020D7FDC01}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{2F6D4BB4-3AAA-44AF-B831-637AF6E9102C}" name="Nombre de la Subred" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{16E39F29-503F-4705-BC1C-506DCA53FE84}" name="Cantidad de Hosts" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{F2CC28B8-4F81-4E26-850E-30A3B60244A5}" name="Dirección de red" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{16E2EFF8-148F-4DA2-867D-D344CD0B901E}" name="Primera IP" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{3FFF7D76-3E36-44F8-88B3-6C82C83089CC}" name="Ultima Ip" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{3A55AF0E-F619-4A07-93C3-9DB9ED50BAB0}" name="BroadCast" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{A52675E2-5FBA-4FB2-B6EB-58BBC7099532}" name="Mascara de Subred" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3651EECB-7826-4B85-9793-CBDC1613CE69}" name="Tabla2" displayName="Tabla2" ref="B20:H23" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="B20:H23" xr:uid="{3651EECB-7826-4B85-9793-CBDC1613CE69}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{2C2F901C-0E0B-4C43-9E89-CDCD9D386FC1}" name="Nombre de la Subred" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{20427634-703A-4FE8-B481-B5FA7BC6DAA2}" name="Cantidad de Hosts" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{969D8931-5F9D-450C-856A-F6D27380D986}" name="Dirección de red" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{AFFA4CBB-C47D-4EDE-8513-5F2F0999C232}" name="Primera IP" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{CE2D76E0-30B2-43EF-BD34-3D8A14584171}" name="Ultima Ip" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{EF5B1524-B69A-4680-90A8-E57DF3CD2115}" name="BroadCast" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{4E9D7CCE-6465-4B2D-8FD9-69B44CDF74B1}" name="Mascara de Subred" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -711,7 +1105,7 @@
   <dimension ref="B2:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +1122,7 @@
   <sheetData>
     <row r="2" spans="2:9" ht="35.25" x14ac:dyDescent="0.5">
       <c r="D2" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="23.25" x14ac:dyDescent="0.3">
@@ -861,7 +1255,7 @@
         <v>37</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>39</v>
@@ -973,13 +1367,13 @@
         <v>53</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="H14" s="5">
         <v>255255255128</v>
@@ -996,13 +1390,13 @@
         <v>58</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="H15" s="5">
         <v>255255255192</v>
@@ -1039,7 +1433,7 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1071,22 +1465,22 @@
     </row>
     <row r="21" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C21" s="5">
         <v>2</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H21" s="5">
         <v>255255255252</v>
@@ -1094,22 +1488,22 @@
     </row>
     <row r="22" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C22" s="5">
         <v>2</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H22" s="5">
         <v>255255255252</v>
@@ -1117,22 +1511,22 @@
     </row>
     <row r="23" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C23" s="5">
         <v>2</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H23" s="5">
         <v>255255255252</v>
@@ -1437,5 +1831,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add www in serveres
</commit_message>
<xml_diff>
--- a/VLSM-VLAN-WAN-CASO-ESTUDIO.xlsx
+++ b/VLSM-VLAN-WAN-CASO-ESTUDIO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Octavo-Semestre\Redes\Caso_De_Estudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D761285-A7DE-47C3-AEF8-70B67BCDB689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF9D1FE-5503-4F61-844D-5FD41F56336D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{70712092-6E08-405F-915F-8AB6473FB4D8}"/>
+    <workbookView xWindow="285" yWindow="435" windowWidth="20205" windowHeight="10365" xr2:uid="{70712092-6E08-405F-915F-8AB6473FB4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1463,7 +1463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>65</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>255255255252</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>66</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>255255255252</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>67</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>255255255252</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="4"/>
@@ -1541,7 +1541,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="4"/>
@@ -1550,7 +1550,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="4"/>
@@ -1559,7 +1559,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="4"/>
@@ -1568,7 +1568,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="4"/>
@@ -1577,7 +1577,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="4"/>
@@ -1586,7 +1586,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1595,7 +1595,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="24" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>

</xml_diff>

<commit_message>
mejoras y new files
</commit_message>
<xml_diff>
--- a/VLSM-VLAN-WAN-CASO-ESTUDIO.xlsx
+++ b/VLSM-VLAN-WAN-CASO-ESTUDIO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Octavo-Semestre\Redes\Caso_De_Estudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF9D1FE-5503-4F61-844D-5FD41F56336D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A760F2-2725-4FAA-9827-938908AE96BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="435" windowWidth="20205" windowHeight="10365" xr2:uid="{70712092-6E08-405F-915F-8AB6473FB4D8}"/>
+    <workbookView xWindow="285" yWindow="390" windowWidth="20205" windowHeight="10365" xr2:uid="{70712092-6E08-405F-915F-8AB6473FB4D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1104,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA0E4DC-57A2-4BCE-8B0D-CB54FA5F8B14}">
   <dimension ref="B2:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add files in packet tracert
</commit_message>
<xml_diff>
--- a/VLSM-VLAN-WAN-CASO-ESTUDIO.xlsx
+++ b/VLSM-VLAN-WAN-CASO-ESTUDIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Octavo-Semestre\Redes\Caso_De_Estudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A760F2-2725-4FAA-9827-938908AE96BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1974FDB-6F1B-4B8A-BB9D-59F4CEB8B5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="390" windowWidth="20205" windowHeight="10365" xr2:uid="{70712092-6E08-405F-915F-8AB6473FB4D8}"/>
   </bookViews>
@@ -1105,7 +1105,7 @@
   <dimension ref="B2:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>